<commit_message>
fix the pds small template
</commit_message>
<xml_diff>
--- a/backend/templates/pds_template.xlsx
+++ b/backend/templates/pds_template.xlsx
@@ -5206,51 +5206,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18820" name="AutoShape 116">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084490000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="11677650" y="2638425"/>
-          <a:ext cx="2314575" cy="1066800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
@@ -10117,8 +10072,8 @@
   </sheetPr>
   <dimension ref="A1:S264"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34:F34"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15583,8 +15538,8 @@
     <hyperlink ref="Q61" r:id="rId205" display="http://www.state.gov/p/eur/ci/ez/"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.15" right="0.12" top="0.36" bottom="0.12" header="0.24" footer="0.12"/>
-  <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId206"/>
+  <pageMargins left="0.15748031496062992" right="0" top="0.15748031496062992" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="5" scale="86" orientation="portrait" r:id="rId206"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId207"/>
   <legacyDrawing r:id="rId208"/>
@@ -15868,7 +15823,7 @@
   </sheetPr>
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A40" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="A48" sqref="A1:M48"/>
     </sheetView>
   </sheetViews>
@@ -16803,8 +16758,8 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.15" right="0" top="0.17" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId2"/>
+  <pageMargins left="0.15748031496062992" right="0" top="0.15748031496062992" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="5" scale="92" orientation="portrait" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -16816,7 +16771,7 @@
   </sheetPr>
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -17650,8 +17605,8 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.17" right="0" top="0.37" bottom="0" header="0.3" footer="0"/>
-  <pageSetup paperSize="9" scale="72" orientation="portrait" r:id="rId2"/>
+  <pageMargins left="0.15748031496062992" right="0" top="0.35433070866141736" bottom="0" header="0.31496062992125984" footer="0"/>
+  <pageSetup paperSize="5" scale="81" orientation="portrait" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -18974,7 +18929,7 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.12" right="0" top="0.34" bottom="0" header="0.17" footer="0"/>
-  <pageSetup paperSize="9" scale="86" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="5" scale="97" orientation="portrait" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>

</xml_diff>